<commit_message>
feat: nuevos datos de prueba
</commit_message>
<xml_diff>
--- a/backend/db/data/empresa.xlsx
+++ b/backend/db/data/empresa.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="35">
   <si>
     <t>razon_social</t>
   </si>
@@ -39,12 +39,6 @@
     <t>comuna</t>
   </si>
   <si>
-    <t>correo</t>
-  </si>
-  <si>
-    <t>fono</t>
-  </si>
-  <si>
     <t>CENCOSUD S.A.</t>
   </si>
   <si>
@@ -57,9 +51,6 @@
     <t>maipu</t>
   </si>
   <si>
-    <t>waveissuttusi-5784@yopmail.com</t>
-  </si>
-  <si>
     <t>COMIDAS  INC.</t>
   </si>
   <si>
@@ -69,9 +60,6 @@
     <t>las condes</t>
   </si>
   <si>
-    <t>ronneurauffiproi-8532@yopmail.com</t>
-  </si>
-  <si>
     <t>PC INC.</t>
   </si>
   <si>
@@ -81,9 +69,6 @@
     <t>la florida</t>
   </si>
   <si>
-    <t>jeulleproiroido-5960@yopmail.com</t>
-  </si>
-  <si>
     <t>ASD INC.</t>
   </si>
   <si>
@@ -93,9 +78,6 @@
     <t>puente alto</t>
   </si>
   <si>
-    <t>fuprarusefa-5444@yopmail.com</t>
-  </si>
-  <si>
     <t>LOLAZO CORP.</t>
   </si>
   <si>
@@ -105,87 +87,61 @@
     <t>cerrillos</t>
   </si>
   <si>
-    <t>rufuvoufrofa-5039@yopmail.com</t>
-  </si>
-  <si>
     <t>DAMX</t>
   </si>
   <si>
     <t>12042938-8</t>
   </si>
   <si>
-    <t>kameffovammau-6049@yopmail.com</t>
-  </si>
-  <si>
     <t>SIZAS</t>
   </si>
   <si>
     <t>5512061-7</t>
   </si>
   <si>
-    <t>gequedusone-5337@yopmail.com</t>
-  </si>
-  <si>
     <t>FASHION</t>
   </si>
   <si>
     <t>12383337-6</t>
   </si>
   <si>
-    <t>youbreidducipoi-2724@yopmail.com</t>
-  </si>
-  <si>
     <t>HAMBRE</t>
   </si>
   <si>
     <t>11465004-8</t>
   </si>
   <si>
-    <t>kequiceibaheu-1123@yopmail.com</t>
-  </si>
-  <si>
     <t>LALA</t>
   </si>
   <si>
     <t>20054447-1</t>
   </si>
   <si>
-    <t>naveyedodda-9082@yopmail.com</t>
-  </si>
-  <si>
     <t>JAJAS</t>
   </si>
   <si>
     <t>2212234-2</t>
-  </si>
-  <si>
-    <t>xdxd@xd.xd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
-      <sz val="10.0"/>
+      <sz val="12.0"/>
       <color theme="1"/>
-      <name val="Verdana"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="12.0"/>
       <color rgb="FF212223"/>
-      <name val="Open Sans"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="18.0"/>
@@ -193,9 +149,9 @@
       <name val="Verdana"/>
     </font>
     <font>
-      <u/>
-      <sz val="11.0"/>
+      <sz val="12.0"/>
       <color theme="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -226,23 +182,20 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -473,316 +426,297 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="H1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="6">
-        <v>9.79597732E8</v>
-      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="5"/>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="6">
-        <v>9.58368398E8</v>
-      </c>
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="5"/>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" s="6">
-        <v>9.09712698E8</v>
-      </c>
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="5"/>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="6">
-        <v>9.52679538E8</v>
-      </c>
+      <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="5"/>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I6" s="6">
-        <v>9.01637474E8</v>
-      </c>
+      <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="5"/>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="A7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I7" s="6">
-        <v>9.04104086E8</v>
-      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="5"/>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I8" s="6">
-        <v>9.56001278E8</v>
-      </c>
+      <c r="A8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="5"/>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I9" s="6">
-        <v>9.32062226E8</v>
-      </c>
+      <c r="A9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="5"/>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I10" s="6">
-        <v>9.63494904E8</v>
-      </c>
+      <c r="A10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="5"/>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I11" s="6">
-        <v>9.03138739E8</v>
-      </c>
+      <c r="A11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="5"/>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="2" t="s">
+      <c r="A12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I12" s="2">
-        <v>1.23456789E8</v>
-      </c>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>
@@ -1765,12 +1699,9 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink r:id="rId1" ref="H3"/>
-  </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>